<commit_message>
prepare data for seasons 19 and 21, import data done
</commit_message>
<xml_diff>
--- a/Team_names.xlsx
+++ b/Team_names.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\PycharmProjects\Masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84637B8A-40F3-4909-9357-1DA99B7664D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D79256-2E84-4BDE-AC52-E01B68E661EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -468,10 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,7 +496,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -510,7 +511,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -525,7 +526,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -540,7 +541,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -555,7 +556,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -570,7 +571,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -585,7 +586,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -600,7 +601,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -615,7 +616,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -630,7 +631,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -675,7 +676,7 @@
         <v>Ja</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -765,7 +766,7 @@
         <v>Ja</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -780,7 +781,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -795,7 +796,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -810,7 +811,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -825,7 +826,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -840,7 +841,7 @@
         <v>Nein</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -856,11 +857,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C25" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C25">
-      <sortCondition ref="C1:C25"/>
-    </sortState>
+  <autoFilter ref="A1:D25" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Ja"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>